<commit_message>
Added demographic data tab to the rating scheme
</commit_message>
<xml_diff>
--- a/rating-scheme.xlsx
+++ b/rating-scheme.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\workspace\phd\students\openapi-evaluation\empirical-evaluation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\workspace\phd\students\openapi-evaluation\openapi-maintainability-benchmark\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1683A3A-F1EE-4FAC-99E7-673DAD0087CD}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="-120" windowWidth="28080" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="840" yWindow="-120" windowWidth="28080" windowHeight="16440"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabellenblatt1" sheetId="1" r:id="rId1"/>
+    <sheet name="schema" sheetId="1" r:id="rId1"/>
+    <sheet name="demographics" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="29">
   <si>
     <t>Complexity</t>
   </si>
@@ -72,16 +72,58 @@
   </si>
   <si>
     <t>TomTom Search</t>
+  </si>
+  <si>
+    <t>Demographic Data</t>
+  </si>
+  <si>
+    <t>strongly disagree</t>
+  </si>
+  <si>
+    <t>disagree</t>
+  </si>
+  <si>
+    <t>neutral</t>
+  </si>
+  <si>
+    <t>agree</t>
+  </si>
+  <si>
+    <t>strongly agree</t>
+  </si>
+  <si>
+    <t>Your current role (e.g. software engineer):</t>
+  </si>
+  <si>
+    <t>Years of professional experience:</t>
+  </si>
+  <si>
+    <t>I am familiar with RESTful web services.</t>
+  </si>
+  <si>
+    <t>I am familiar with the OpenAPI specification.</t>
+  </si>
+  <si>
+    <t>I am familiar with the WSDL specification.</t>
+  </si>
+  <si>
+    <t>I am familiar with service orientation in general.</t>
+  </si>
+  <si>
+    <t>I am familiar with Microservices.</t>
+  </si>
+  <si>
+    <t>I am familiar with software quality assurance.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#0"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -116,6 +158,25 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="13"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -306,10 +367,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -343,17 +406,25 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -664,14 +735,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:G111"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -682,10 +753,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="17"/>
+      <c r="B1" s="18"/>
     </row>
     <row r="2" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -708,7 +779,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="20" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="9" t="s">
@@ -728,7 +799,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="19"/>
+      <c r="A6" s="20"/>
       <c r="B6" s="10" t="s">
         <v>3</v>
       </c>
@@ -738,7 +809,7 @@
       <c r="F6" s="5"/>
     </row>
     <row r="7" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="20" t="s">
+      <c r="A7" s="21" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="9" t="s">
@@ -758,7 +829,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="20"/>
+      <c r="A8" s="21"/>
       <c r="B8" s="10" t="s">
         <v>3</v>
       </c>
@@ -768,7 +839,7 @@
       <c r="F8" s="5"/>
     </row>
     <row r="9" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="20" t="s">
+      <c r="A9" s="21" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="9" t="s">
@@ -788,7 +859,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="20"/>
+      <c r="A10" s="21"/>
       <c r="B10" s="10" t="s">
         <v>3</v>
       </c>
@@ -798,7 +869,7 @@
       <c r="F10" s="5"/>
     </row>
     <row r="11" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="20" t="s">
+      <c r="A11" s="21" t="s">
         <v>10</v>
       </c>
       <c r="B11" s="9" t="s">
@@ -818,7 +889,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="20"/>
+      <c r="A12" s="21"/>
       <c r="B12" s="10" t="s">
         <v>3</v>
       </c>
@@ -828,7 +899,7 @@
       <c r="F12" s="5"/>
     </row>
     <row r="13" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="20" t="s">
+      <c r="A13" s="21" t="s">
         <v>11</v>
       </c>
       <c r="B13" s="9" t="s">
@@ -848,7 +919,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="20"/>
+      <c r="A14" s="21"/>
       <c r="B14" s="10" t="s">
         <v>3</v>
       </c>
@@ -858,7 +929,7 @@
       <c r="F14" s="5"/>
     </row>
     <row r="15" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="20" t="s">
+      <c r="A15" s="21" t="s">
         <v>12</v>
       </c>
       <c r="B15" s="9" t="s">
@@ -878,7 +949,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="20"/>
+      <c r="A16" s="21"/>
       <c r="B16" s="10" t="s">
         <v>3</v>
       </c>
@@ -888,7 +959,7 @@
       <c r="F16" s="5"/>
     </row>
     <row r="17" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="20" t="s">
+      <c r="A17" s="21" t="s">
         <v>13</v>
       </c>
       <c r="B17" s="9" t="s">
@@ -908,7 +979,7 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="20"/>
+      <c r="A18" s="21"/>
       <c r="B18" s="10" t="s">
         <v>3</v>
       </c>
@@ -918,7 +989,7 @@
       <c r="F18" s="5"/>
     </row>
     <row r="19" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="20" t="s">
+      <c r="A19" s="21" t="s">
         <v>14</v>
       </c>
       <c r="B19" s="9" t="s">
@@ -938,11 +1009,11 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="20"/>
+      <c r="A20" s="21"/>
       <c r="B20" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C20" s="18"/>
+      <c r="C20" s="17"/>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
       <c r="F20" s="5"/>
@@ -1024,8 +1095,134 @@
     <mergeCell ref="A11:A12"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error" error="Value must be between 1 and 10_x000a_" sqref="C17:F17 C15:F15 C13:F13 C11:F11 C9:F9 C7:F7 C5:F5 C19:F19" xr:uid="{156B71DA-2A4C-44AC-85EC-280C7C88BD08}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error" error="Value must be between 1 and 10_x000a_" sqref="C17:F17 C15:F15 C13:F13 C11:F11 C9:F9 C7:F7 C5:F5 C19:F19">
       <formula1>$A$102:$A$111</formula1>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="A5:A6" r:id="rId1" display="Amazon Transcribe Service"/>
+    <hyperlink ref="A7:A8" r:id="rId2" display="BBC iPlayer"/>
+    <hyperlink ref="A9:A10" r:id="rId3" display="BBC Nitro"/>
+    <hyperlink ref="A11:A12" r:id="rId4" display="Google Apps Customer Management"/>
+    <hyperlink ref="A13:A14" r:id="rId5" display="Government of British Columbia: Job Postings"/>
+    <hyperlink ref="A15:A16" r:id="rId6" display="TomTom Maps"/>
+    <hyperlink ref="A17:A18" r:id="rId7" display="TomTom Routing"/>
+    <hyperlink ref="A19:A20" r:id="rId8" display="TomTom Search"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1:B99"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="40.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.7109375" customWidth="1"/>
+    <col min="3" max="3" width="25.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A1" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="18"/>
+    </row>
+    <row r="2" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="19"/>
+    </row>
+    <row r="7" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="22" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="22" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="19" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="19" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="22" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="95" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A95" s="19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A96" s="19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A97" s="19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A98" s="19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A99" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7:B12">
+      <formula1>$A$95:$A$99</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>